<commit_message>
Fix altair renderer and pin packages' versions
</commit_message>
<xml_diff>
--- a/out/pocos_ABL.xlsx
+++ b/out/pocos_ABL.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plan1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -57,19 +57,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -699,7 +699,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -914,7 +914,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1336,7 +1336,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -2341,7 +2341,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -2552,7 +2552,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -3752,7 +3752,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -4745,7 +4745,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -4944,7 +4944,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -5141,7 +5141,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -5342,7 +5342,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>ABL  </t>
+          <t xml:space="preserve">ABL  </t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -5510,6 +5510,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>